<commit_message>
add some and delete the repeate
</commit_message>
<xml_diff>
--- a/abstruction/论文.xlsx
+++ b/abstruction/论文.xlsx
@@ -203,9 +203,6 @@
     <t>传统三维建模扫描技术通常使用结构光扫描仪或者激光扫描仪获得高精度数据，用以生成高真实感的三维虚拟人个性化模型[2]。</t>
   </si>
   <si>
-    <t>Cyberware 人体扫描系统[3]市面报价为24 万元，普通用户很难承受如此价格。此外，Cyberware 等设备均要求用户保持一定时间的静止状态，如Cyberware 的捕获时间为17 秒</t>
-  </si>
-  <si>
     <t>Tong et al.[7]借助了三台Kinect 完成人体的捕获。但是，该系统需要大约30 秒的数据采集时间，而且，文献[7]的系统还需要转盘等设备。这严重限制了重建系统的适用范围。</t>
   </si>
   <si>
@@ -300,6 +297,10 @@
   </si>
   <si>
     <t>相对于一般静态物体或场景的扫描重建 10-14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cyberware 人体扫描系统[3]市面报价为24 万元，普通用户很难承受如此价格。此外，Cyberware 等设备均要求用户保持一定时间的静止状态，如Cyberware 的捕获时间为17 秒</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6769,8 +6770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6871,7 +6872,7 @@
     <row r="13" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>50</v>
@@ -6880,37 +6881,37 @@
     <row r="14" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -6921,82 +6922,82 @@
     <row r="19" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="8"/>
     </row>
@@ -7009,42 +7010,42 @@
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>